<commit_message>
Added 'north wind' units as cognate pairs, updated measures accordingly
</commit_message>
<xml_diff>
--- a/Multilingual Cloze Tests/Distances/Multilingual_Story_Alignments.xlsx
+++ b/Multilingual Cloze Tests/Distances/Multilingual_Story_Alignments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phgeorgis/Documents/Work/HiWi/Multilingual Cloze Tests/Distances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F98420-20CC-8D4D-ACA8-9DC91FE38861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF79CBF0-EA25-2C42-B3D9-F7E80940F8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{50D3A534-966A-B444-99D7-50AE72F8F7BC}"/>
   </bookViews>
@@ -3290,9 +3290,6 @@
     <t>Północny Wiatr</t>
   </si>
   <si>
-    <t>Severni  veter</t>
-  </si>
-  <si>
     <t>Sjeverni vjetar</t>
   </si>
   <si>
@@ -3333,6 +3330,9 @@
   </si>
   <si>
     <t xml:space="preserve">pʲiʋˈnʲiʧnɪi̯ ˈʋitɛr </t>
+  </si>
+  <si>
+    <t>Severni veter</t>
   </si>
 </sst>
 </file>
@@ -3847,8 +3847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE950C2F-C0E1-9A4C-AD2A-CC9DB6905229}">
   <dimension ref="A1:AP76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4146,7 +4146,7 @@
         <v>408</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>1084</v>
+        <v>1098</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>434</v>
@@ -4187,7 +4187,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>25</v>
@@ -4232,7 +4232,7 @@
         <v>46</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>2</v>
@@ -5670,7 +5670,7 @@
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="E41" s="16" t="s">
-        <v>1084</v>
+        <v>1098</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="16" t="s">
@@ -5746,7 +5746,7 @@
         <v>231</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="16" t="s">
@@ -5825,7 +5825,7 @@
         <v>239</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>240</v>
@@ -6074,7 +6074,7 @@
       </c>
       <c r="F52" s="16"/>
       <c r="G52" s="16" t="s">
-        <v>1084</v>
+        <v>1098</v>
       </c>
       <c r="H52" s="16"/>
       <c r="I52" s="16"/>
@@ -6101,7 +6101,7 @@
       </c>
       <c r="F53" s="16"/>
       <c r="G53" s="25" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="H53" s="16"/>
       <c r="I53" s="16"/>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="F54" s="16"/>
       <c r="G54" s="16" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
@@ -6910,7 +6910,7 @@
         <v>37</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>1084</v>
+        <v>1098</v>
       </c>
       <c r="G74" s="7" t="s">
         <v>411</v>
@@ -6947,7 +6947,7 @@
       <c r="B75" s="16"/>
       <c r="C75" s="16"/>
       <c r="F75" s="25" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="H75" s="16"/>
       <c r="I75" s="17" t="s">
@@ -6996,7 +6996,7 @@
         <v>330</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H76" s="16"/>
       <c r="J76" s="16"/>
@@ -9696,8 +9696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E57938-4EF9-7247-85CC-24C28FE07AE3}">
   <dimension ref="A1:AP76"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9759,7 +9759,7 @@
         <v>561</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>562</v>
@@ -9792,7 +9792,7 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>562</v>
@@ -9844,7 +9844,7 @@
         <v>562</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="K4" s="16"/>
       <c r="O4" s="16" t="s">
@@ -9877,7 +9877,7 @@
         <v>586</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>562</v>
@@ -9997,7 +9997,7 @@
         <v>408</v>
       </c>
       <c r="G8" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>434</v>
@@ -10038,7 +10038,7 @@
         <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>25</v>
@@ -10083,7 +10083,7 @@
         <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>562</v>
@@ -11088,7 +11088,7 @@
         <v>813</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>814</v>
@@ -11162,7 +11162,7 @@
         <v>835</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="G36" s="16"/>
       <c r="H36" s="16"/>
@@ -11231,7 +11231,7 @@
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
       <c r="E37" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
@@ -11300,7 +11300,7 @@
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
       <c r="E38" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>868</v>
@@ -11521,7 +11521,7 @@
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="E41" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="16" t="s">
@@ -11597,7 +11597,7 @@
         <v>935</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="16" t="s">
@@ -11676,7 +11676,7 @@
         <v>949</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>950</v>
@@ -11760,7 +11760,7 @@
       </c>
       <c r="F46" s="16"/>
       <c r="G46" s="16" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H46" s="16" t="s">
         <v>829</v>
@@ -11793,7 +11793,7 @@
       </c>
       <c r="F47" s="16"/>
       <c r="G47" s="16" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="H47" s="16"/>
       <c r="I47" s="16"/>
@@ -11820,7 +11820,7 @@
       </c>
       <c r="F48" s="16"/>
       <c r="G48" s="16" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="H48" s="16"/>
       <c r="I48" s="16"/>
@@ -11844,7 +11844,7 @@
       </c>
       <c r="F49" s="16"/>
       <c r="G49" s="16" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="H49" s="16"/>
       <c r="I49" s="16"/>
@@ -11925,7 +11925,7 @@
       </c>
       <c r="F52" s="16"/>
       <c r="G52" s="16" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="H52" s="16"/>
       <c r="I52" s="16"/>
@@ -11952,7 +11952,7 @@
       </c>
       <c r="F53" s="16"/>
       <c r="G53" s="16" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="H53" s="16"/>
       <c r="I53" s="16"/>
@@ -11974,7 +11974,7 @@
       </c>
       <c r="F54" s="16"/>
       <c r="G54" s="16" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
@@ -12511,7 +12511,7 @@
         <v>1028</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H68" s="16"/>
       <c r="J68" s="16"/>
@@ -12548,7 +12548,7 @@
         <v>1034</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="H69" s="16"/>
       <c r="J69" s="16"/>
@@ -12595,7 +12595,7 @@
         <v>1042</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="H70" s="16"/>
       <c r="J70" s="16"/>
@@ -12642,7 +12642,7 @@
         <v>1049</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="G71" s="15" t="s">
         <v>1050</v>
@@ -12761,7 +12761,7 @@
         <v>608</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G74" s="7" t="s">
         <v>1062</v>
@@ -12798,7 +12798,7 @@
       <c r="B75" s="16"/>
       <c r="C75" s="16"/>
       <c r="F75" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="H75" s="16"/>
       <c r="I75" s="17" t="s">
@@ -12847,7 +12847,7 @@
         <v>1071</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="H76" s="16"/>
       <c r="J76" s="16"/>

</xml_diff>